<commit_message>
Added required java libraries
</commit_message>
<xml_diff>
--- a/templates.xlsx
+++ b/templates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vhulendamoraba/Desktop/Course/Project/DAFT/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3161ADC3-8B18-AA41-88E6-5EF224090D71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333F79D8-496F-5141-AB1B-27DA2D93B99D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-32000" yWindow="0" windowWidth="32000" windowHeight="18000" xr2:uid="{FC74CED3-F350-9947-896C-EF9DBB7A60A9}"/>
   </bookViews>
@@ -66,20 +66,6 @@
     <t>Title (Bank charges)</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Uchithe iningi lemali yakho </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;subCategory1&gt;, &lt;subCategory2&gt;, &lt;subCategory3&gt;, &lt;subCategory4&gt;.</t>
-    </r>
-  </si>
-  <si>
     <t>Title (Budget on track)</t>
   </si>
   <si>
@@ -119,6 +105,9 @@
   </si>
   <si>
     <t>weqe isabelomali sakho sokusetshenziswa ngamarandi ${Amount} ezidingweni n${Amount2} ezintweni zokunethezeka</t>
+  </si>
+  <si>
+    <t>izindleko zakho eziphakeme kakhulu ${subCategory1}, ${subCategory2}, ${subCategory3} ${na}${subCategory4}.</t>
   </si>
 </sst>
 </file>
@@ -514,8 +503,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872ED92F-00A6-6448-99E7-7295FE151D1F}">
   <dimension ref="A1:AH21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>6</v>
@@ -562,13 +551,13 @@
     </row>
     <row r="2" spans="1:34" ht="40" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>4</v>
@@ -577,16 +566,16 @@
         <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>

</xml_diff>